<commit_message>
ex-247 (jebene) edited functional test
</commit_message>
<xml_diff>
--- a/test/functional_tests/translate_to_excel/expected_output.xlsx
+++ b/test/functional_tests/translate_to_excel/expected_output.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>gene symbol</t>
   </si>
   <si>
-    <t>PATIENT_A</t>
+    <t>PATIENT_A_SnpEff</t>
+  </si>
+  <si>
+    <t>PATIENT_A_dbNSFP</t>
   </si>
   <si>
     <t>SnpEff_overall_impact_rank</t>
@@ -44,7 +47,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,14 +71,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF6699FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="4"/>
       <color rgb="FF003366"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF003366"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -90,7 +107,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFA500"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF003366"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -122,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -130,6 +159,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,13 +455,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,33 +471,43 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ex-249 (jebene) began setting up dbNSFP and SnpEff to return a list of style dataframes
</commit_message>
<xml_diff>
--- a/test/functional_tests/translate_to_excel/expected_output.xlsx
+++ b/test/functional_tests/translate_to_excel/expected_output.xlsx
@@ -72,7 +72,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF6699FF"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,7 +92,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,13 +113,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF003366"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -151,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -159,8 +165,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,7 +493,7 @@
       <c r="C2" s="4">
         <v>12</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="5">
         <v>2</v>
       </c>
     </row>
@@ -501,13 +509,13 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>4</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="8">
         <v>1</v>
       </c>
     </row>

</xml_diff>